<commit_message>
celery reddis pipeline and dummy frontend
</commit_message>
<xml_diff>
--- a/assets/csv/results/gate_verification_results.xlsx
+++ b/assets/csv/results/gate_verification_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -543,793 +543,649 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1007</t>
+          <t>1002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tonmoya.sarmah@example.com</t>
+          <t>anupam.chowdhury@example.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+91-9123456789</t>
+          <t>+91-8765432109</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>TONMOYA SARMAH</t>
+          <t>Anupam Chowdhury</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tonmoya Sarmah</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'The candidate's name is Anupam Chowdhury.'</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CS17S64003076</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>CS17S64003076</t>
-        </is>
-      </c>
+          <t>TF16S84009003</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>428</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>428</t>
-        </is>
-      </c>
+          <t>557</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>31.99</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>31.99</t>
-        </is>
-      </c>
+          <t>36.33</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>6844</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>6844.</t>
-        </is>
-      </c>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1002</t>
+          <t>1003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>anupam.chowdhury@example.com</t>
+          <t>kumar.aman@example.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>+91-8765432109</t>
+          <t>+91-7654321098</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Anupam Chowdhury</t>
+          <t>KUMAR AMAN</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ANUPAM CHOWDHURY</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'The candidate name is Kumar Aman.'</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>TF16S84009003</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>TF16S84009003</t>
-        </is>
-      </c>
+          <t>CE19S74019008</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>557</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>557</t>
-        </is>
-      </c>
+          <t>754</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>36.33</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>36.33</t>
-        </is>
-      </c>
+          <t>63.96</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>69</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>69.</t>
-        </is>
-      </c>
+          <t>661</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1013</t>
+          <t>1004</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>shakir.ahmad.bhat@example.com</t>
+          <t>kunal.pradhan@example.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>+91-9789012345</t>
+          <t>+91-9012345678</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SHAKIR AHMAD BHAT</t>
+          <t>KUNAL PRADHAN</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Shakir Ahmad Bhat</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'The candidate's name is Kunal Pradhan.'</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CE19S83051160</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>CE19S83051160</t>
-        </is>
-      </c>
+          <t>CS17S56065411</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>352</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>352</t>
-        </is>
-      </c>
+          <t>394</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>28.36</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>28.36</t>
-        </is>
-      </c>
+          <t>28.9</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>20407</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>20407.</t>
-        </is>
-      </c>
+          <t>8751</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1008</t>
+          <t>1005</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>shruti.umarvaish@example.com</t>
+          <t>najmul.haque.barbhuiya@example.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>+91-8234567890</t>
+          <t>+91-8901234567</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SHRUTI UMARVAISH</t>
+          <t>NAJMUL HAQUE BARBHUIYA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SHRUTI UMARVAISH</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'NAJMUL HAQUE BARBHUIYA.'</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>BT21S56005123</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>BT21S56005123</t>
-        </is>
-      </c>
+          <t>CE17S84018058</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>541</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>541</t>
-        </is>
-      </c>
+          <t>554</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>43</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
+          <t>48.26</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>426</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>426.</t>
-        </is>
-      </c>
+          <t>4350</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1011</t>
+          <t>1006</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ankur.agrawal@example.com</t>
+          <t>rukaiya.khatoon@example.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>+91-8567890123</t>
+          <t>+91-7890123456</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ankur Agrawal</t>
+          <t>RUKAIYA KHATOON</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Ankur Agrawal</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'The candidate's name is Rukaiya Khatoon.'</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ME19S11228033</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>ME19S11228033</t>
-        </is>
-      </c>
+          <t>PH16S26070056</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>902</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>902</t>
-        </is>
-      </c>
+          <t>491</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>85.49</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>85.49</t>
-        </is>
-      </c>
+          <t>45.33</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>65</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>65.</t>
-        </is>
-      </c>
+          <t>608</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1003</t>
+          <t>1007</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>kumar.aman@example.com</t>
+          <t>tonmoya.sarmah@example.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>+91-7654321098</t>
+          <t>+91-9123456789</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>KUMAR AMAN</t>
+          <t>TONMOYA SARMAH</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>KUMAR AMAN</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'The candidate name is Tonmoya Sarmah.'</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>CE19S74019008</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>CE19S74019008</t>
-        </is>
-      </c>
+          <t>CS17S64003076</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>754</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>754</t>
-        </is>
-      </c>
+          <t>428</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>63.96</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>63.96</t>
-        </is>
-      </c>
+          <t>31.99</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>661</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>661.</t>
-        </is>
-      </c>
+          <t>6844</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1005</t>
+          <t>1008</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>najmul.haque.barbhuiya@example.com</t>
+          <t>shruti.umarvaish@example.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>+91-8901234567</t>
+          <t>+91-8234567890</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NAJMUL HAQUE BARBHUIYA</t>
+          <t>SHRUTI UMARVAISH</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>NAJMUL HAQUE BARBHUIYA</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'The candidate name is Shruti Umarvaish.'</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>CE17S84018058</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>CE17S84018058</t>
-        </is>
-      </c>
+          <t>BT21S56005123</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>554</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>554</t>
-        </is>
-      </c>
+          <t>541</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>48.26</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>48.26</t>
-        </is>
-      </c>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>4350</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>4350.</t>
-        </is>
-      </c>
+          <t>426</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1006</t>
+          <t>1011</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>rukaiya.khatoon@example.com</t>
+          <t>ankur.agrawal@example.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>+91-7890123456</t>
+          <t>+91-8567890123</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>RUKAIYA KHATOON</t>
+          <t>Ankur Agrawal</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>RUKAIYA KHATOON</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: '**Candidate Name:** Ankur Agrawal'</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>PH16S26070056</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>PH16526070056</t>
-        </is>
-      </c>
+          <t>ME19S11228033</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>False</t>
@@ -1337,169 +1193,133 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>491</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>491</t>
-        </is>
-      </c>
+          <t>902</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>45.33</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>45.33</t>
-        </is>
-      </c>
+          <t>85.49</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>608</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>608.</t>
-        </is>
-      </c>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1004</t>
+          <t>1013</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>kunal.pradhan@example.com</t>
+          <t>shakir.ahmad.bhat@example.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>+91-9012345678</t>
+          <t>+91-9789012345</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>KUNAL PRADHAN</t>
+          <t>SHAKIR AHMAD BHAT</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Kunal Pradhan</t>
+          <t>PARSE_ERROR: Expected 6 fields, got 1. Raw: 'The candidate name is SHAKIR AHMAD BHAT.'</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>CS17S56065411</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>CS17S56065411</t>
-        </is>
-      </c>
+          <t>CE19S83051160</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>394</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>394</t>
-        </is>
-      </c>
+          <t>352</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>28.9</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>28.9</t>
-        </is>
-      </c>
+          <t>28.36</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>8751</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>8751.</t>
-        </is>
-      </c>
+          <t>20407</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>

</xml_diff>